<commit_message>
add `transpose` option in table module
</commit_message>
<xml_diff>
--- a/test/xlsx-connector/test.xlsx
+++ b/test/xlsx-connector/test.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D13D363-01D9-4ADF-A5D1-1F3007FDC0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="s1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>a</t>
   </si>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -103,7 +104,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -111,14 +112,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -156,7 +160,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -228,7 +232,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -401,19 +405,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -459,7 +463,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -476,7 +480,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -496,28 +500,112 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>7654</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
replace `_set` to `setProperty`
</commit_message>
<xml_diff>
--- a/test/xlsx-connector/test.xlsx
+++ b/test/xlsx-connector/test.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D13D363-01D9-4ADF-A5D1-1F3007FDC0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E207256-770C-44DC-91D2-543B5F30F5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="s1" sheetId="1" r:id="rId1"/>
@@ -55,16 +55,16 @@
     <t>555 ;</t>
   </si>
   <si>
-    <t>one.1</t>
-  </si>
-  <si>
     <t>we</t>
   </si>
   <si>
     <t>rt</t>
   </si>
   <si>
-    <t>z.0</t>
+    <t>one[1]</t>
+  </si>
+  <si>
+    <t>z[0]</t>
   </si>
 </sst>
 </file>
@@ -408,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,7 +434,7 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
         <v>15</v>
@@ -457,10 +457,10 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,10 +578,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -589,7 +589,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>